<commit_message>
23/09/25 - lần 3
</commit_message>
<xml_diff>
--- a/tests/Result/Result_Xlsx_test_search.xlsx
+++ b/tests/Result/Result_Xlsx_test_search.xlsx
@@ -481,7 +481,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
     </row>
@@ -506,7 +506,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
     </row>

</xml_diff>